<commit_message>
interface evaluation added and interface better
</commit_message>
<xml_diff>
--- a/BD_results_poligrafo.xlsx
+++ b/BD_results_poligrafo.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karan\Desktop\FakeNews-App\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3224FFB5-4927-452A-8B9B-DED8474CCE73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="113">
   <si>
     <t>Label</t>
   </si>
@@ -64,12 +70,6 @@
     <t>social</t>
   </si>
   <si>
-    <t xml:space="preserve">Verdadeiro </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Falso </t>
-  </si>
-  <si>
     <t>3.6</t>
   </si>
   <si>
@@ -290,13 +290,82 @@
   </si>
   <si>
     <t>21.4</t>
+  </si>
+  <si>
+    <t>strongsubj</t>
+  </si>
+  <si>
+    <t>weaksubj</t>
+  </si>
+  <si>
+    <t>valence_avg</t>
+  </si>
+  <si>
+    <t>valence_std</t>
+  </si>
+  <si>
+    <t>valence_max</t>
+  </si>
+  <si>
+    <t>valence_min</t>
+  </si>
+  <si>
+    <t>valence_dif</t>
+  </si>
+  <si>
+    <t>arousal_avg</t>
+  </si>
+  <si>
+    <t>arousal_std</t>
+  </si>
+  <si>
+    <t>arousal_max</t>
+  </si>
+  <si>
+    <t>arousal_min</t>
+  </si>
+  <si>
+    <t>arousal_dif</t>
+  </si>
+  <si>
+    <t>dominance_avg</t>
+  </si>
+  <si>
+    <t>dominance_std</t>
+  </si>
+  <si>
+    <t>dominance_max</t>
+  </si>
+  <si>
+    <t>dominance_min</t>
+  </si>
+  <si>
+    <t>dominance_dif</t>
+  </si>
+  <si>
+    <t>Alegria</t>
+  </si>
+  <si>
+    <t>Desgosto</t>
+  </si>
+  <si>
+    <t>Medo</t>
+  </si>
+  <si>
+    <t>Raiva</t>
+  </si>
+  <si>
+    <t>Surpresa</t>
+  </si>
+  <si>
+    <t>Tristeza</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,11 +402,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -379,7 +456,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,9 +488,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -445,6 +540,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -620,14 +733,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AM31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -676,10 +791,79 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" t="s">
+        <v>107</v>
+      </c>
+      <c r="R1" t="s">
+        <v>108</v>
+      </c>
+      <c r="S1" t="s">
+        <v>109</v>
+      </c>
+      <c r="T1" t="s">
+        <v>110</v>
+      </c>
+      <c r="U1" t="s">
+        <v>111</v>
+      </c>
+      <c r="V1" t="s">
+        <v>112</v>
+      </c>
+      <c r="W1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>106</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>16</v>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -688,19 +872,19 @@
         <v>12.1</v>
       </c>
       <c r="D2">
-        <v>5.623</v>
+        <v>5.6230000000000002</v>
       </c>
       <c r="E2">
-        <v>4.123</v>
+        <v>4.1230000000000002</v>
       </c>
       <c r="F2">
-        <v>5.478</v>
+        <v>5.4779999999999998</v>
       </c>
       <c r="G2">
         <v>3.6</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -718,18 +902,87 @@
         <v>37.1</v>
       </c>
       <c r="N2">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="O2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P2" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>7</v>
+      </c>
+      <c r="X2">
+        <v>10</v>
+      </c>
+      <c r="Y2">
+        <v>5.6230000000000002</v>
+      </c>
+      <c r="Z2">
+        <v>1.1653</v>
+      </c>
+      <c r="AA2">
+        <v>7.68</v>
+      </c>
+      <c r="AB2">
+        <v>2.85</v>
+      </c>
+      <c r="AC2">
+        <v>4.83</v>
+      </c>
+      <c r="AD2">
+        <v>4.1230000000000002</v>
+      </c>
+      <c r="AE2">
+        <v>0.75280000000000002</v>
+      </c>
+      <c r="AF2">
+        <v>5.8</v>
+      </c>
+      <c r="AG2">
+        <v>2.9</v>
+      </c>
+      <c r="AH2">
+        <v>2.9</v>
+      </c>
+      <c r="AI2">
+        <v>5.4779999999999998</v>
+      </c>
+      <c r="AJ2">
+        <v>0.68110000000000004</v>
+      </c>
+      <c r="AK2">
+        <v>6.61</v>
+      </c>
+      <c r="AL2">
+        <v>3.78</v>
+      </c>
+      <c r="AM2">
+        <v>2.83</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>16</v>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
       </c>
       <c r="B3">
         <v>5.2</v>
@@ -738,7 +991,7 @@
         <v>25</v>
       </c>
       <c r="D3">
-        <v>5.544</v>
+        <v>5.5439999999999996</v>
       </c>
       <c r="E3">
         <v>4.117</v>
@@ -750,7 +1003,7 @@
         <v>4.2</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -771,15 +1024,84 @@
         <v>11.5</v>
       </c>
       <c r="O3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P3" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="Q3">
+        <v>60</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>20</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>20</v>
+      </c>
+      <c r="W3">
+        <v>8</v>
+      </c>
+      <c r="X3">
+        <v>16</v>
+      </c>
+      <c r="Y3">
+        <v>5.5439999999999996</v>
+      </c>
+      <c r="Z3">
+        <v>1.1217999999999999</v>
+      </c>
+      <c r="AA3">
+        <v>7.22</v>
+      </c>
+      <c r="AB3">
+        <v>2.33</v>
+      </c>
+      <c r="AC3">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="AD3">
+        <v>4.117</v>
+      </c>
+      <c r="AE3">
+        <v>0.76470000000000005</v>
+      </c>
+      <c r="AF3">
+        <v>5.79</v>
+      </c>
+      <c r="AG3">
+        <v>2.98</v>
+      </c>
+      <c r="AH3">
+        <v>2.81</v>
+      </c>
+      <c r="AI3">
+        <v>5.649</v>
+      </c>
+      <c r="AJ3">
+        <v>0.61839999999999995</v>
+      </c>
+      <c r="AK3">
+        <v>6.86</v>
+      </c>
+      <c r="AL3">
+        <v>3.95</v>
+      </c>
+      <c r="AM3">
+        <v>2.91</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
-        <v>16</v>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -788,19 +1110,19 @@
         <v>18.2</v>
       </c>
       <c r="D4">
-        <v>5.309</v>
+        <v>5.3090000000000002</v>
       </c>
       <c r="E4">
-        <v>3.973</v>
+        <v>3.9729999999999999</v>
       </c>
       <c r="F4">
-        <v>5.736</v>
+        <v>5.7359999999999998</v>
       </c>
       <c r="G4">
         <v>4.5</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -815,21 +1137,90 @@
         <v>27.3</v>
       </c>
       <c r="M4">
-        <v>54.50000000000001</v>
+        <v>54.500000000000007</v>
       </c>
       <c r="N4">
         <v>11.4</v>
       </c>
       <c r="O4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P4" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>8</v>
+      </c>
+      <c r="Y4">
+        <v>5.3090000000000002</v>
+      </c>
+      <c r="Z4">
+        <v>0.92110000000000003</v>
+      </c>
+      <c r="AA4">
+        <v>7.86</v>
+      </c>
+      <c r="AB4">
+        <v>3.71</v>
+      </c>
+      <c r="AC4">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="AD4">
+        <v>3.9729999999999999</v>
+      </c>
+      <c r="AE4">
+        <v>0.68130000000000002</v>
+      </c>
+      <c r="AF4">
+        <v>6.26</v>
+      </c>
+      <c r="AG4">
+        <v>3</v>
+      </c>
+      <c r="AH4">
+        <v>3.26</v>
+      </c>
+      <c r="AI4">
+        <v>5.7359999999999998</v>
+      </c>
+      <c r="AJ4">
+        <v>0.92810000000000004</v>
+      </c>
+      <c r="AK4">
+        <v>7.11</v>
+      </c>
+      <c r="AL4">
+        <v>3.71</v>
+      </c>
+      <c r="AM4">
+        <v>3.4</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5" t="s">
-        <v>16</v>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
       </c>
       <c r="B5">
         <v>5.3</v>
@@ -838,10 +1229,10 @@
         <v>14.5</v>
       </c>
       <c r="D5">
-        <v>5.214</v>
+        <v>5.2140000000000004</v>
       </c>
       <c r="E5">
-        <v>3.841</v>
+        <v>3.8410000000000002</v>
       </c>
       <c r="F5">
         <v>5.827</v>
@@ -850,7 +1241,7 @@
         <v>5.3</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -871,15 +1262,84 @@
         <v>14.5</v>
       </c>
       <c r="O5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P5" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="Q5">
+        <v>25</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>75</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>3</v>
+      </c>
+      <c r="X5">
+        <v>8</v>
+      </c>
+      <c r="Y5">
+        <v>5.2140000000000004</v>
+      </c>
+      <c r="Z5">
+        <v>1.0254000000000001</v>
+      </c>
+      <c r="AA5">
+        <v>7.16</v>
+      </c>
+      <c r="AB5">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AC5">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="AD5">
+        <v>3.8410000000000002</v>
+      </c>
+      <c r="AE5">
+        <v>0.54820000000000002</v>
+      </c>
+      <c r="AF5">
+        <v>5.36</v>
+      </c>
+      <c r="AG5">
+        <v>3</v>
+      </c>
+      <c r="AH5">
+        <v>2.36</v>
+      </c>
+      <c r="AI5">
+        <v>5.827</v>
+      </c>
+      <c r="AJ5">
+        <v>0.87709999999999999</v>
+      </c>
+      <c r="AK5">
+        <v>7.39</v>
+      </c>
+      <c r="AL5">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="AM5">
+        <v>4.92</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" t="s">
-        <v>16</v>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
       </c>
       <c r="B6">
         <v>4.2</v>
@@ -888,10 +1348,10 @@
         <v>20.8</v>
       </c>
       <c r="D6">
-        <v>5.148</v>
+        <v>5.1479999999999997</v>
       </c>
       <c r="E6">
-        <v>4.015</v>
+        <v>4.0149999999999997</v>
       </c>
       <c r="F6">
         <v>5.383</v>
@@ -900,7 +1360,7 @@
         <v>1.8</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -921,15 +1381,84 @@
         <v>11.9</v>
       </c>
       <c r="O6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="P6" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="Q6">
+        <v>28.57</v>
+      </c>
+      <c r="R6">
+        <v>28.57</v>
+      </c>
+      <c r="S6">
+        <v>14.29</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>28.57</v>
+      </c>
+      <c r="W6">
+        <v>14</v>
+      </c>
+      <c r="X6">
+        <v>21</v>
+      </c>
+      <c r="Y6">
+        <v>5.1479999999999997</v>
+      </c>
+      <c r="Z6">
+        <v>1.3015000000000001</v>
+      </c>
+      <c r="AA6">
+        <v>7.5</v>
+      </c>
+      <c r="AB6">
+        <v>1.72</v>
+      </c>
+      <c r="AC6">
+        <v>5.78</v>
+      </c>
+      <c r="AD6">
+        <v>4.0149999999999997</v>
+      </c>
+      <c r="AE6">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AF6">
+        <v>5.45</v>
+      </c>
+      <c r="AG6">
+        <v>2.57</v>
+      </c>
+      <c r="AH6">
+        <v>2.88</v>
+      </c>
+      <c r="AI6">
+        <v>5.383</v>
+      </c>
+      <c r="AJ6">
+        <v>0.94420000000000004</v>
+      </c>
+      <c r="AK6">
+        <v>7.33</v>
+      </c>
+      <c r="AL6">
+        <v>3.08</v>
+      </c>
+      <c r="AM6">
+        <v>4.25</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
-      <c r="A7" t="s">
-        <v>16</v>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
       </c>
       <c r="B7">
         <v>1.3</v>
@@ -938,10 +1467,10 @@
         <v>8.4</v>
       </c>
       <c r="D7">
-        <v>5.294</v>
+        <v>5.2939999999999996</v>
       </c>
       <c r="E7">
-        <v>3.983</v>
+        <v>3.9830000000000001</v>
       </c>
       <c r="F7">
         <v>5.49</v>
@@ -950,7 +1479,7 @@
         <v>2.6</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -965,21 +1494,90 @@
         <v>32.9</v>
       </c>
       <c r="M7">
-        <v>19.4</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="N7">
         <v>5.2</v>
       </c>
       <c r="O7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P7" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>100</v>
+      </c>
+      <c r="W7">
+        <v>6</v>
+      </c>
+      <c r="X7">
+        <v>7</v>
+      </c>
+      <c r="Y7">
+        <v>5.2939999999999996</v>
+      </c>
+      <c r="Z7">
+        <v>0.74980000000000002</v>
+      </c>
+      <c r="AA7">
+        <v>6.79</v>
+      </c>
+      <c r="AB7">
+        <v>3.78</v>
+      </c>
+      <c r="AC7">
+        <v>3.01</v>
+      </c>
+      <c r="AD7">
+        <v>3.9830000000000001</v>
+      </c>
+      <c r="AE7">
+        <v>0.6724</v>
+      </c>
+      <c r="AF7">
+        <v>5.73</v>
+      </c>
+      <c r="AG7">
+        <v>2.64</v>
+      </c>
+      <c r="AH7">
+        <v>3.09</v>
+      </c>
+      <c r="AI7">
+        <v>5.49</v>
+      </c>
+      <c r="AJ7">
+        <v>0.6593</v>
+      </c>
+      <c r="AK7">
+        <v>6.74</v>
+      </c>
+      <c r="AL7">
+        <v>3.11</v>
+      </c>
+      <c r="AM7">
+        <v>3.63</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8" t="s">
-        <v>16</v>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
       </c>
       <c r="B8">
         <v>3.4</v>
@@ -988,19 +1586,19 @@
         <v>20.9</v>
       </c>
       <c r="D8">
-        <v>5.377</v>
+        <v>5.3769999999999998</v>
       </c>
       <c r="E8">
         <v>4.141</v>
       </c>
       <c r="F8">
-        <v>5.567</v>
+        <v>5.5670000000000002</v>
       </c>
       <c r="G8">
         <v>5.3</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -1009,7 +1607,7 @@
         <v>1</v>
       </c>
       <c r="K8">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="L8">
         <v>23.8</v>
@@ -1018,18 +1616,87 @@
         <v>46.6</v>
       </c>
       <c r="N8">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="O8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P8" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="Q8">
+        <v>50</v>
+      </c>
+      <c r="R8">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="S8">
+        <v>33.33</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>13</v>
+      </c>
+      <c r="X8">
+        <v>30</v>
+      </c>
+      <c r="Y8">
+        <v>5.3769999999999998</v>
+      </c>
+      <c r="Z8">
+        <v>1.2173</v>
+      </c>
+      <c r="AA8">
+        <v>7.68</v>
+      </c>
+      <c r="AB8">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AC8">
+        <v>5.63</v>
+      </c>
+      <c r="AD8">
+        <v>4.141</v>
+      </c>
+      <c r="AE8">
+        <v>0.73519999999999996</v>
+      </c>
+      <c r="AF8">
+        <v>6.31</v>
+      </c>
+      <c r="AG8">
+        <v>2.98</v>
+      </c>
+      <c r="AH8">
+        <v>3.33</v>
+      </c>
+      <c r="AI8">
+        <v>5.5670000000000002</v>
+      </c>
+      <c r="AJ8">
+        <v>0.91159999999999997</v>
+      </c>
+      <c r="AK8">
+        <v>7.22</v>
+      </c>
+      <c r="AL8">
+        <v>2.58</v>
+      </c>
+      <c r="AM8">
+        <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
-      <c r="A9" t="s">
-        <v>16</v>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
       </c>
       <c r="B9">
         <v>3.6</v>
@@ -1038,10 +1705,10 @@
         <v>16.3</v>
       </c>
       <c r="D9">
-        <v>5.119</v>
+        <v>5.1189999999999998</v>
       </c>
       <c r="E9">
-        <v>4.143</v>
+        <v>4.1429999999999998</v>
       </c>
       <c r="F9">
         <v>5.375</v>
@@ -1050,7 +1717,7 @@
         <v>4.8</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1062,7 +1729,7 @@
         <v>5.4</v>
       </c>
       <c r="L9">
-        <v>35.8</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="M9">
         <v>38.9</v>
@@ -1071,36 +1738,105 @@
         <v>14.8</v>
       </c>
       <c r="O9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P9" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="Q9">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="R9">
+        <v>41.67</v>
+      </c>
+      <c r="S9">
+        <v>33.33</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>8.33</v>
+      </c>
+      <c r="W9">
+        <v>23</v>
+      </c>
+      <c r="X9">
+        <v>31</v>
+      </c>
+      <c r="Y9">
+        <v>5.1189999999999998</v>
+      </c>
+      <c r="Z9">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AA9">
+        <v>7.73</v>
+      </c>
+      <c r="AB9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AC9">
+        <v>5.43</v>
+      </c>
+      <c r="AD9">
+        <v>4.1429999999999998</v>
+      </c>
+      <c r="AE9">
+        <v>0.8397</v>
+      </c>
+      <c r="AF9">
+        <v>6.59</v>
+      </c>
+      <c r="AG9">
+        <v>1.97</v>
+      </c>
+      <c r="AH9">
+        <v>4.62</v>
+      </c>
+      <c r="AI9">
+        <v>5.375</v>
+      </c>
+      <c r="AJ9">
+        <v>0.88680000000000003</v>
+      </c>
+      <c r="AK9">
+        <v>7.29</v>
+      </c>
+      <c r="AL9">
+        <v>3.17</v>
+      </c>
+      <c r="AM9">
+        <v>4.12</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
-      <c r="A10" t="s">
-        <v>16</v>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
       </c>
       <c r="B10">
         <v>2.7</v>
       </c>
       <c r="C10">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="D10">
-        <v>5.324</v>
+        <v>5.3239999999999998</v>
       </c>
       <c r="E10">
         <v>4.03</v>
       </c>
       <c r="F10">
-        <v>5.427</v>
+        <v>5.4269999999999996</v>
       </c>
       <c r="G10">
         <v>3.6</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1121,15 +1857,84 @@
         <v>14.3</v>
       </c>
       <c r="O10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P10" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="Q10">
+        <v>66.67</v>
+      </c>
+      <c r="R10">
+        <v>33.33</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>9</v>
+      </c>
+      <c r="X10">
+        <v>11</v>
+      </c>
+      <c r="Y10">
+        <v>5.3239999999999998</v>
+      </c>
+      <c r="Z10">
+        <v>1.0995999999999999</v>
+      </c>
+      <c r="AA10">
+        <v>7.76</v>
+      </c>
+      <c r="AB10">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="AC10">
+        <v>5.48</v>
+      </c>
+      <c r="AD10">
+        <v>4.03</v>
+      </c>
+      <c r="AE10">
+        <v>0.64710000000000001</v>
+      </c>
+      <c r="AF10">
+        <v>5.79</v>
+      </c>
+      <c r="AG10">
+        <v>2.85</v>
+      </c>
+      <c r="AH10">
+        <v>2.94</v>
+      </c>
+      <c r="AI10">
+        <v>5.4269999999999996</v>
+      </c>
+      <c r="AJ10">
+        <v>0.69240000000000002</v>
+      </c>
+      <c r="AK10">
+        <v>6.54</v>
+      </c>
+      <c r="AL10">
+        <v>3.7</v>
+      </c>
+      <c r="AM10">
+        <v>2.84</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
-      <c r="A11" t="s">
-        <v>16</v>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
       </c>
       <c r="B11">
         <v>6.9</v>
@@ -1138,19 +1943,19 @@
         <v>21.2</v>
       </c>
       <c r="D11">
-        <v>5.455</v>
+        <v>5.4550000000000001</v>
       </c>
       <c r="E11">
-        <v>4.227</v>
+        <v>4.2270000000000003</v>
       </c>
       <c r="F11">
-        <v>5.597</v>
+        <v>5.5970000000000004</v>
       </c>
       <c r="G11">
-        <v>4.399999999999999</v>
+        <v>4.3999999999999986</v>
       </c>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -1159,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>4.399999999999999</v>
+        <v>4.3999999999999986</v>
       </c>
       <c r="L11">
         <v>26.9</v>
@@ -1171,15 +1976,84 @@
         <v>20</v>
       </c>
       <c r="O11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P11" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="Q11">
+        <v>85.71</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>14.29</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>17</v>
+      </c>
+      <c r="X11">
+        <v>17</v>
+      </c>
+      <c r="Y11">
+        <v>5.4550000000000001</v>
+      </c>
+      <c r="Z11">
+        <v>1.07</v>
+      </c>
+      <c r="AA11">
+        <v>7.86</v>
+      </c>
+      <c r="AB11">
+        <v>2.4</v>
+      </c>
+      <c r="AC11">
+        <v>5.46</v>
+      </c>
+      <c r="AD11">
+        <v>4.2270000000000003</v>
+      </c>
+      <c r="AE11">
+        <v>0.90629999999999999</v>
+      </c>
+      <c r="AF11">
+        <v>6.26</v>
+      </c>
+      <c r="AG11">
+        <v>2.19</v>
+      </c>
+      <c r="AH11">
+        <v>4.07</v>
+      </c>
+      <c r="AI11">
+        <v>5.5970000000000004</v>
+      </c>
+      <c r="AJ11">
+        <v>0.79549999999999998</v>
+      </c>
+      <c r="AK11">
+        <v>7.26</v>
+      </c>
+      <c r="AL11">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="AM11">
+        <v>4.83</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
-      <c r="A12" t="s">
-        <v>16</v>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
       </c>
       <c r="B12">
         <v>5.5</v>
@@ -1188,10 +2062,10 @@
         <v>14.7</v>
       </c>
       <c r="D12">
-        <v>5.542</v>
+        <v>5.5419999999999998</v>
       </c>
       <c r="E12">
-        <v>3.921</v>
+        <v>3.9209999999999998</v>
       </c>
       <c r="F12">
         <v>5.556</v>
@@ -1200,7 +2074,7 @@
         <v>6</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -1221,15 +2095,84 @@
         <v>20.3</v>
       </c>
       <c r="O12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P12" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="Q12">
+        <v>22.22</v>
+      </c>
+      <c r="R12">
+        <v>11.11</v>
+      </c>
+      <c r="S12">
+        <v>11.11</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>11.11</v>
+      </c>
+      <c r="V12">
+        <v>44.44</v>
+      </c>
+      <c r="W12">
+        <v>8</v>
+      </c>
+      <c r="X12">
+        <v>24</v>
+      </c>
+      <c r="Y12">
+        <v>5.5419999999999998</v>
+      </c>
+      <c r="Z12">
+        <v>1.0382</v>
+      </c>
+      <c r="AA12">
+        <v>7.33</v>
+      </c>
+      <c r="AB12">
+        <v>3</v>
+      </c>
+      <c r="AC12">
+        <v>4.33</v>
+      </c>
+      <c r="AD12">
+        <v>3.9209999999999998</v>
+      </c>
+      <c r="AE12">
+        <v>0.64970000000000006</v>
+      </c>
+      <c r="AF12">
+        <v>5.83</v>
+      </c>
+      <c r="AG12">
+        <v>2.5</v>
+      </c>
+      <c r="AH12">
+        <v>3.33</v>
+      </c>
+      <c r="AI12">
+        <v>5.556</v>
+      </c>
+      <c r="AJ12">
+        <v>0.86270000000000002</v>
+      </c>
+      <c r="AK12">
+        <v>7.35</v>
+      </c>
+      <c r="AL12">
+        <v>3.05</v>
+      </c>
+      <c r="AM12">
+        <v>4.3</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
-      <c r="A13" t="s">
-        <v>16</v>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
       </c>
       <c r="B13">
         <v>3.2</v>
@@ -1241,7 +2184,7 @@
         <v>5.101</v>
       </c>
       <c r="E13">
-        <v>4.237</v>
+        <v>4.2370000000000001</v>
       </c>
       <c r="F13">
         <v>5.306</v>
@@ -1250,7 +2193,7 @@
         <v>3.2</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1268,18 +2211,87 @@
         <v>52.8</v>
       </c>
       <c r="N13">
-        <v>18.4</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="O13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P13" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="Q13">
+        <v>50</v>
+      </c>
+      <c r="R13">
+        <v>25</v>
+      </c>
+      <c r="S13">
+        <v>25</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>8</v>
+      </c>
+      <c r="X13">
+        <v>13</v>
+      </c>
+      <c r="Y13">
+        <v>5.101</v>
+      </c>
+      <c r="Z13">
+        <v>1.1645000000000001</v>
+      </c>
+      <c r="AA13">
+        <v>7.52</v>
+      </c>
+      <c r="AB13">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="AC13">
+        <v>4.99</v>
+      </c>
+      <c r="AD13">
+        <v>4.2370000000000001</v>
+      </c>
+      <c r="AE13">
+        <v>0.7097</v>
+      </c>
+      <c r="AF13">
+        <v>5.71</v>
+      </c>
+      <c r="AG13">
+        <v>2.5</v>
+      </c>
+      <c r="AH13">
+        <v>3.21</v>
+      </c>
+      <c r="AI13">
+        <v>5.306</v>
+      </c>
+      <c r="AJ13">
+        <v>1.0106999999999999</v>
+      </c>
+      <c r="AK13">
+        <v>7</v>
+      </c>
+      <c r="AL13">
+        <v>3</v>
+      </c>
+      <c r="AM13">
+        <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" t="s">
-        <v>16</v>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
       </c>
       <c r="B14">
         <v>5.7</v>
@@ -1288,19 +2300,19 @@
         <v>23.3</v>
       </c>
       <c r="D14">
-        <v>5.205</v>
+        <v>5.2050000000000001</v>
       </c>
       <c r="E14">
-        <v>4.238</v>
+        <v>4.2380000000000004</v>
       </c>
       <c r="F14">
-        <v>5.439</v>
+        <v>5.4390000000000001</v>
       </c>
       <c r="G14">
-        <v>4.399999999999999</v>
+        <v>4.3999999999999986</v>
       </c>
       <c r="H14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1312,7 +2324,7 @@
         <v>5</v>
       </c>
       <c r="L14">
-        <v>35.8</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="M14">
         <v>45.3</v>
@@ -1321,15 +2333,84 @@
         <v>13.2</v>
       </c>
       <c r="O14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P14" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="Q14">
+        <v>12.5</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>25</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>62.5</v>
+      </c>
+      <c r="W14">
+        <v>14</v>
+      </c>
+      <c r="X14">
+        <v>23</v>
+      </c>
+      <c r="Y14">
+        <v>5.2050000000000001</v>
+      </c>
+      <c r="Z14">
+        <v>1.3244</v>
+      </c>
+      <c r="AA14">
+        <v>7.57</v>
+      </c>
+      <c r="AB14">
+        <v>1.91</v>
+      </c>
+      <c r="AC14">
+        <v>5.66</v>
+      </c>
+      <c r="AD14">
+        <v>4.2380000000000004</v>
+      </c>
+      <c r="AE14">
+        <v>0.88849999999999996</v>
+      </c>
+      <c r="AF14">
+        <v>6.71</v>
+      </c>
+      <c r="AG14">
+        <v>2.5</v>
+      </c>
+      <c r="AH14">
+        <v>4.21</v>
+      </c>
+      <c r="AI14">
+        <v>5.4390000000000001</v>
+      </c>
+      <c r="AJ14">
+        <v>0.98829999999999996</v>
+      </c>
+      <c r="AK14">
+        <v>7.21</v>
+      </c>
+      <c r="AL14">
+        <v>1.95</v>
+      </c>
+      <c r="AM14">
+        <v>5.26</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
-      <c r="A15" t="s">
-        <v>16</v>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
       </c>
       <c r="B15">
         <v>3.4</v>
@@ -1338,19 +2419,19 @@
         <v>18</v>
       </c>
       <c r="D15">
-        <v>5.254</v>
+        <v>5.2539999999999996</v>
       </c>
       <c r="E15">
-        <v>4.045</v>
+        <v>4.0449999999999999</v>
       </c>
       <c r="F15">
-        <v>5.206</v>
+        <v>5.2060000000000004</v>
       </c>
       <c r="G15">
         <v>3.9</v>
       </c>
       <c r="H15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1359,48 +2440,117 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <v>5.600000000000001</v>
+        <v>5.6000000000000014</v>
       </c>
       <c r="L15">
         <v>28.9</v>
       </c>
       <c r="M15">
-        <v>36.8</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="N15">
         <v>8.6</v>
       </c>
       <c r="O15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="P15" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q15">
+        <v>25</v>
+      </c>
+      <c r="R15">
+        <v>8.33</v>
+      </c>
+      <c r="S15">
+        <v>25</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>41.67</v>
+      </c>
+      <c r="W15">
+        <v>27</v>
+      </c>
+      <c r="X15">
         <v>57</v>
       </c>
+      <c r="Y15">
+        <v>5.2539999999999996</v>
+      </c>
+      <c r="Z15">
+        <v>1.1608000000000001</v>
+      </c>
+      <c r="AA15">
+        <v>7.79</v>
+      </c>
+      <c r="AB15">
+        <v>1.9</v>
+      </c>
+      <c r="AC15">
+        <v>5.89</v>
+      </c>
+      <c r="AD15">
+        <v>4.0449999999999999</v>
+      </c>
+      <c r="AE15">
+        <v>0.91459999999999997</v>
+      </c>
+      <c r="AF15">
+        <v>6.6</v>
+      </c>
+      <c r="AG15">
+        <v>2.19</v>
+      </c>
+      <c r="AH15">
+        <v>4.41</v>
+      </c>
+      <c r="AI15">
+        <v>5.2060000000000004</v>
+      </c>
+      <c r="AJ15">
+        <v>0.83819999999999995</v>
+      </c>
+      <c r="AK15">
+        <v>7.63</v>
+      </c>
+      <c r="AL15">
+        <v>2.9</v>
+      </c>
+      <c r="AM15">
+        <v>4.7300000000000004</v>
+      </c>
     </row>
-    <row r="16" spans="1:16">
-      <c r="A16" t="s">
-        <v>16</v>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
       </c>
       <c r="B16">
-        <v>8.200000000000001</v>
+        <v>8.2000000000000011</v>
       </c>
       <c r="C16">
         <v>20.3</v>
       </c>
       <c r="D16">
-        <v>4.979</v>
+        <v>4.9790000000000001</v>
       </c>
       <c r="E16">
-        <v>4.378</v>
+        <v>4.3780000000000001</v>
       </c>
       <c r="F16">
-        <v>5.253</v>
+        <v>5.2530000000000001</v>
       </c>
       <c r="G16">
         <v>3.8</v>
       </c>
       <c r="H16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -1409,7 +2559,7 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>5.600000000000001</v>
+        <v>5.6000000000000014</v>
       </c>
       <c r="L16">
         <v>30.5</v>
@@ -1421,36 +2571,105 @@
         <v>11.7</v>
       </c>
       <c r="O16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P16" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="Q16">
+        <v>7.02</v>
+      </c>
+      <c r="R16">
+        <v>3.51</v>
+      </c>
+      <c r="S16">
+        <v>31.58</v>
+      </c>
+      <c r="T16">
+        <v>21.05</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>36.840000000000003</v>
+      </c>
+      <c r="W16">
+        <v>60</v>
+      </c>
+      <c r="X16">
+        <v>84</v>
+      </c>
+      <c r="Y16">
+        <v>4.9790000000000001</v>
+      </c>
+      <c r="Z16">
+        <v>1.3122</v>
+      </c>
+      <c r="AA16">
+        <v>7.73</v>
+      </c>
+      <c r="AB16">
+        <v>1.89</v>
+      </c>
+      <c r="AC16">
+        <v>5.84</v>
+      </c>
+      <c r="AD16">
+        <v>4.3780000000000001</v>
+      </c>
+      <c r="AE16">
+        <v>1.0368999999999999</v>
+      </c>
+      <c r="AF16">
+        <v>7.37</v>
+      </c>
+      <c r="AG16">
+        <v>2.19</v>
+      </c>
+      <c r="AH16">
+        <v>5.18</v>
+      </c>
+      <c r="AI16">
+        <v>5.2530000000000001</v>
+      </c>
+      <c r="AJ16">
+        <v>1.0286999999999999</v>
+      </c>
+      <c r="AK16">
+        <v>7.42</v>
+      </c>
+      <c r="AL16">
+        <v>2.64</v>
+      </c>
+      <c r="AM16">
+        <v>4.78</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
-      <c r="A17" t="s">
-        <v>17</v>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
       </c>
       <c r="B17">
         <v>3.5</v>
       </c>
       <c r="C17">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="D17">
-        <v>5.623</v>
+        <v>5.6230000000000002</v>
       </c>
       <c r="E17">
-        <v>4.071</v>
+        <v>4.0709999999999997</v>
       </c>
       <c r="F17">
-        <v>5.612</v>
+        <v>5.6120000000000001</v>
       </c>
       <c r="G17">
         <v>3.8</v>
       </c>
       <c r="H17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -1471,15 +2690,84 @@
         <v>15</v>
       </c>
       <c r="O17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="P17" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="Q17">
+        <v>40</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>10</v>
+      </c>
+      <c r="T17">
+        <v>10</v>
+      </c>
+      <c r="U17">
+        <v>10</v>
+      </c>
+      <c r="V17">
+        <v>30</v>
+      </c>
+      <c r="W17">
+        <v>17</v>
+      </c>
+      <c r="X17">
+        <v>35</v>
+      </c>
+      <c r="Y17">
+        <v>5.6230000000000002</v>
+      </c>
+      <c r="Z17">
+        <v>1.0206</v>
+      </c>
+      <c r="AA17">
+        <v>7.68</v>
+      </c>
+      <c r="AB17">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AC17">
+        <v>5.13</v>
+      </c>
+      <c r="AD17">
+        <v>4.0709999999999997</v>
+      </c>
+      <c r="AE17">
+        <v>0.7641</v>
+      </c>
+      <c r="AF17">
+        <v>6.6</v>
+      </c>
+      <c r="AG17">
+        <v>2.71</v>
+      </c>
+      <c r="AH17">
+        <v>3.89</v>
+      </c>
+      <c r="AI17">
+        <v>5.6120000000000001</v>
+      </c>
+      <c r="AJ17">
+        <v>0.71479999999999999</v>
+      </c>
+      <c r="AK17">
+        <v>6.96</v>
+      </c>
+      <c r="AL17">
+        <v>2.56</v>
+      </c>
+      <c r="AM17">
+        <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
-      <c r="A18" t="s">
-        <v>17</v>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
       </c>
       <c r="B18">
         <v>6.7</v>
@@ -1500,7 +2788,7 @@
         <v>2.5</v>
       </c>
       <c r="H18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -1509,7 +2797,7 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <v>4.399999999999999</v>
+        <v>4.3999999999999986</v>
       </c>
       <c r="L18">
         <v>30.3</v>
@@ -1521,15 +2809,84 @@
         <v>15.9</v>
       </c>
       <c r="O18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P18" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="Q18">
+        <v>39.47</v>
+      </c>
+      <c r="R18">
+        <v>5.26</v>
+      </c>
+      <c r="S18">
+        <v>2.63</v>
+      </c>
+      <c r="T18">
+        <v>23.68</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>28.95</v>
+      </c>
+      <c r="W18">
+        <v>39</v>
+      </c>
+      <c r="X18">
+        <v>48</v>
+      </c>
+      <c r="Y18">
+        <v>5.65</v>
+      </c>
+      <c r="Z18">
+        <v>1.3596999999999999</v>
+      </c>
+      <c r="AA18">
+        <v>8.02</v>
+      </c>
+      <c r="AB18">
+        <v>1.91</v>
+      </c>
+      <c r="AC18">
+        <v>6.11</v>
+      </c>
+      <c r="AD18">
+        <v>4.431</v>
+      </c>
+      <c r="AE18">
+        <v>1.0237000000000001</v>
+      </c>
+      <c r="AF18">
+        <v>7.19</v>
+      </c>
+      <c r="AG18">
+        <v>2.44</v>
+      </c>
+      <c r="AH18">
+        <v>4.75</v>
+      </c>
+      <c r="AI18">
+        <v>5.67</v>
+      </c>
+      <c r="AJ18">
+        <v>0.85719999999999996</v>
+      </c>
+      <c r="AK18">
+        <v>7.26</v>
+      </c>
+      <c r="AL18">
+        <v>1.95</v>
+      </c>
+      <c r="AM18">
+        <v>5.31</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
-      <c r="A19" t="s">
-        <v>17</v>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
       </c>
       <c r="B19">
         <v>4.8</v>
@@ -1538,19 +2895,19 @@
         <v>22.8</v>
       </c>
       <c r="D19">
-        <v>5.707</v>
+        <v>5.7069999999999999</v>
       </c>
       <c r="E19">
-        <v>4.225</v>
+        <v>4.2249999999999996</v>
       </c>
       <c r="F19">
-        <v>5.747</v>
+        <v>5.7469999999999999</v>
       </c>
       <c r="G19">
         <v>7.9</v>
       </c>
       <c r="H19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -1571,36 +2928,105 @@
         <v>13.2</v>
       </c>
       <c r="O19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P19" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="Q19">
+        <v>37.5</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>37.5</v>
+      </c>
+      <c r="T19">
+        <v>12.5</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>12.5</v>
+      </c>
+      <c r="W19">
+        <v>17</v>
+      </c>
+      <c r="X19">
+        <v>26</v>
+      </c>
+      <c r="Y19">
+        <v>5.7069999999999999</v>
+      </c>
+      <c r="Z19">
+        <v>1.0844</v>
+      </c>
+      <c r="AA19">
+        <v>7.68</v>
+      </c>
+      <c r="AB19">
+        <v>2.21</v>
+      </c>
+      <c r="AC19">
+        <v>5.47</v>
+      </c>
+      <c r="AD19">
+        <v>4.2249999999999996</v>
+      </c>
+      <c r="AE19">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="AF19">
+        <v>5.95</v>
+      </c>
+      <c r="AG19">
+        <v>2.62</v>
+      </c>
+      <c r="AH19">
+        <v>3.33</v>
+      </c>
+      <c r="AI19">
+        <v>5.7469999999999999</v>
+      </c>
+      <c r="AJ19">
+        <v>0.69269999999999998</v>
+      </c>
+      <c r="AK19">
+        <v>7.42</v>
+      </c>
+      <c r="AL19">
+        <v>3.41</v>
+      </c>
+      <c r="AM19">
+        <v>4.01</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
-      <c r="A20" t="s">
-        <v>17</v>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
       </c>
       <c r="B20">
         <v>7.1</v>
       </c>
       <c r="C20">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="D20">
-        <v>5.363</v>
+        <v>5.3630000000000004</v>
       </c>
       <c r="E20">
-        <v>4.244</v>
+        <v>4.2439999999999998</v>
       </c>
       <c r="F20">
-        <v>5.204</v>
+        <v>5.2039999999999997</v>
       </c>
       <c r="G20">
         <v>3.6</v>
       </c>
       <c r="H20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1621,15 +3047,84 @@
         <v>14.9</v>
       </c>
       <c r="O20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P20" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="Q20">
+        <v>12.5</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>37.5</v>
+      </c>
+      <c r="T20">
+        <v>37.5</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>12.5</v>
+      </c>
+      <c r="W20">
+        <v>8</v>
+      </c>
+      <c r="X20">
+        <v>22</v>
+      </c>
+      <c r="Y20">
+        <v>5.3630000000000004</v>
+      </c>
+      <c r="Z20">
+        <v>1.1515</v>
+      </c>
+      <c r="AA20">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="AB20">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AC20">
+        <v>5.91</v>
+      </c>
+      <c r="AD20">
+        <v>4.2439999999999998</v>
+      </c>
+      <c r="AE20">
+        <v>0.82650000000000001</v>
+      </c>
+      <c r="AF20">
+        <v>6.72</v>
+      </c>
+      <c r="AG20">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="AH20">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AI20">
+        <v>5.2039999999999997</v>
+      </c>
+      <c r="AJ20">
+        <v>0.75929999999999997</v>
+      </c>
+      <c r="AK20">
+        <v>6.9</v>
+      </c>
+      <c r="AL20">
+        <v>2.64</v>
+      </c>
+      <c r="AM20">
+        <v>4.26</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
-      <c r="A21" t="s">
-        <v>17</v>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0</v>
       </c>
       <c r="B21">
         <v>4.7</v>
@@ -1638,10 +3133,10 @@
         <v>13.5</v>
       </c>
       <c r="D21">
-        <v>5.115</v>
+        <v>5.1150000000000002</v>
       </c>
       <c r="E21">
-        <v>4.185</v>
+        <v>4.1849999999999996</v>
       </c>
       <c r="F21">
         <v>5.359</v>
@@ -1650,7 +3145,7 @@
         <v>2.8</v>
       </c>
       <c r="H21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -1668,39 +3163,108 @@
         <v>46</v>
       </c>
       <c r="N21">
-        <v>7.399999999999999</v>
+        <v>7.3999999999999986</v>
       </c>
       <c r="O21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P21" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="Q21">
+        <v>10</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>60</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>30</v>
+      </c>
+      <c r="W21">
+        <v>8</v>
+      </c>
+      <c r="X21">
+        <v>21</v>
+      </c>
+      <c r="Y21">
+        <v>5.1150000000000002</v>
+      </c>
+      <c r="Z21">
+        <v>1.2686999999999999</v>
+      </c>
+      <c r="AA21">
+        <v>7.33</v>
+      </c>
+      <c r="AB21">
+        <v>1.71</v>
+      </c>
+      <c r="AC21">
+        <v>5.62</v>
+      </c>
+      <c r="AD21">
+        <v>4.1849999999999996</v>
+      </c>
+      <c r="AE21">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="AF21">
+        <v>6.72</v>
+      </c>
+      <c r="AG21">
+        <v>2.57</v>
+      </c>
+      <c r="AH21">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="AI21">
+        <v>5.359</v>
+      </c>
+      <c r="AJ21">
+        <v>0.90190000000000003</v>
+      </c>
+      <c r="AK21">
+        <v>7.17</v>
+      </c>
+      <c r="AL21">
+        <v>1.95</v>
+      </c>
+      <c r="AM21">
+        <v>5.22</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
-      <c r="A22" t="s">
-        <v>17</v>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
       </c>
       <c r="B22">
-        <v>4.399999999999999</v>
+        <v>4.3999999999999986</v>
       </c>
       <c r="C22">
         <v>14.8</v>
       </c>
       <c r="D22">
-        <v>4.963</v>
+        <v>4.9630000000000001</v>
       </c>
       <c r="E22">
-        <v>4.323</v>
+        <v>4.3230000000000004</v>
       </c>
       <c r="F22">
-        <v>5.261</v>
+        <v>5.2610000000000001</v>
       </c>
       <c r="G22">
         <v>3.8</v>
       </c>
       <c r="H22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -1712,24 +3276,93 @@
         <v>6</v>
       </c>
       <c r="L22">
-        <v>32.2</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="M22">
-        <v>39.90000000000001</v>
+        <v>39.900000000000013</v>
       </c>
       <c r="N22">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="O22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P22" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>66.67</v>
+      </c>
+      <c r="S22">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="W22">
+        <v>2</v>
+      </c>
+      <c r="X22">
+        <v>25</v>
+      </c>
+      <c r="Y22">
+        <v>4.9630000000000001</v>
+      </c>
+      <c r="Z22">
+        <v>1.1661999999999999</v>
+      </c>
+      <c r="AA22">
+        <v>6.68</v>
+      </c>
+      <c r="AB22">
+        <v>2.33</v>
+      </c>
+      <c r="AC22">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="AD22">
+        <v>4.3230000000000004</v>
+      </c>
+      <c r="AE22">
+        <v>1.0690999999999999</v>
+      </c>
+      <c r="AF22">
+        <v>7.15</v>
+      </c>
+      <c r="AG22">
+        <v>2.85</v>
+      </c>
+      <c r="AH22">
+        <v>4.3</v>
+      </c>
+      <c r="AI22">
+        <v>5.2610000000000001</v>
+      </c>
+      <c r="AJ22">
+        <v>1.0488999999999999</v>
+      </c>
+      <c r="AK22">
+        <v>7.16</v>
+      </c>
+      <c r="AL22">
+        <v>2.56</v>
+      </c>
+      <c r="AM22">
+        <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
-      <c r="A23" t="s">
-        <v>17</v>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0</v>
       </c>
       <c r="B23">
         <v>3.8</v>
@@ -1741,16 +3374,16 @@
         <v>5.431</v>
       </c>
       <c r="E23">
-        <v>4.401</v>
+        <v>4.4009999999999998</v>
       </c>
       <c r="F23">
-        <v>5.822</v>
+        <v>5.8220000000000001</v>
       </c>
       <c r="G23">
         <v>11.3</v>
       </c>
       <c r="H23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -1771,15 +3404,84 @@
         <v>11.3</v>
       </c>
       <c r="O23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P23" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="Q23">
+        <v>100</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>2</v>
+      </c>
+      <c r="X23">
+        <v>7</v>
+      </c>
+      <c r="Y23">
+        <v>5.431</v>
+      </c>
+      <c r="Z23">
+        <v>1.3322000000000001</v>
+      </c>
+      <c r="AA23">
+        <v>7.95</v>
+      </c>
+      <c r="AB23">
+        <v>3.85</v>
+      </c>
+      <c r="AC23">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AD23">
+        <v>4.4009999999999998</v>
+      </c>
+      <c r="AE23">
+        <v>0.94640000000000002</v>
+      </c>
+      <c r="AF23">
+        <v>6.27</v>
+      </c>
+      <c r="AG23">
+        <v>2.62</v>
+      </c>
+      <c r="AH23">
+        <v>3.65</v>
+      </c>
+      <c r="AI23">
+        <v>5.8220000000000001</v>
+      </c>
+      <c r="AJ23">
+        <v>0.71460000000000001</v>
+      </c>
+      <c r="AK23">
+        <v>7</v>
+      </c>
+      <c r="AL23">
+        <v>4.5</v>
+      </c>
+      <c r="AM23">
+        <v>2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
-      <c r="A24" t="s">
-        <v>17</v>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
       </c>
       <c r="B24">
         <v>6.3</v>
@@ -1788,7 +3490,7 @@
         <v>15.9</v>
       </c>
       <c r="D24">
-        <v>5.246</v>
+        <v>5.2460000000000004</v>
       </c>
       <c r="E24">
         <v>4.202</v>
@@ -1800,7 +3502,7 @@
         <v>9.5</v>
       </c>
       <c r="H24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -1812,24 +3514,93 @@
         <v>11.1</v>
       </c>
       <c r="L24">
-        <v>39.7</v>
+        <v>39.700000000000003</v>
       </c>
       <c r="M24">
-        <v>52.40000000000001</v>
+        <v>52.400000000000013</v>
       </c>
       <c r="N24">
         <v>14.3</v>
       </c>
       <c r="O24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P24" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="Q24">
+        <v>25</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>50</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>25</v>
+      </c>
+      <c r="W24">
+        <v>3</v>
+      </c>
+      <c r="X24">
+        <v>7</v>
+      </c>
+      <c r="Y24">
+        <v>5.2460000000000004</v>
+      </c>
+      <c r="Z24">
+        <v>1.2036</v>
+      </c>
+      <c r="AA24">
+        <v>7.73</v>
+      </c>
+      <c r="AB24">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="AC24">
+        <v>5.2</v>
+      </c>
+      <c r="AD24">
+        <v>4.202</v>
+      </c>
+      <c r="AE24">
+        <v>0.67989999999999995</v>
+      </c>
+      <c r="AF24">
+        <v>5.8</v>
+      </c>
+      <c r="AG24">
+        <v>3.25</v>
+      </c>
+      <c r="AH24">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AI24">
+        <v>5.444</v>
+      </c>
+      <c r="AJ24">
+        <v>0.68030000000000002</v>
+      </c>
+      <c r="AK24">
+        <v>6.61</v>
+      </c>
+      <c r="AL24">
+        <v>3.85</v>
+      </c>
+      <c r="AM24">
+        <v>2.76</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
-      <c r="A25" t="s">
-        <v>17</v>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
       </c>
       <c r="B25">
         <v>3.8</v>
@@ -1838,19 +3609,19 @@
         <v>15.1</v>
       </c>
       <c r="D25">
-        <v>5.584</v>
+        <v>5.5839999999999996</v>
       </c>
       <c r="E25">
-        <v>4.365</v>
+        <v>4.3650000000000002</v>
       </c>
       <c r="F25">
-        <v>5.594</v>
+        <v>5.5940000000000003</v>
       </c>
       <c r="G25">
-        <v>6.600000000000001</v>
+        <v>6.6000000000000014</v>
       </c>
       <c r="H25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -1871,15 +3642,84 @@
         <v>19.8</v>
       </c>
       <c r="O25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P25" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="Q25">
+        <v>100</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>4</v>
+      </c>
+      <c r="X25">
+        <v>12</v>
+      </c>
+      <c r="Y25">
+        <v>5.5839999999999996</v>
+      </c>
+      <c r="Z25">
+        <v>1.1416999999999999</v>
+      </c>
+      <c r="AA25">
+        <v>7.38</v>
+      </c>
+      <c r="AB25">
+        <v>1.71</v>
+      </c>
+      <c r="AC25">
+        <v>5.67</v>
+      </c>
+      <c r="AD25">
+        <v>4.3650000000000002</v>
+      </c>
+      <c r="AE25">
+        <v>0.7964</v>
+      </c>
+      <c r="AF25">
+        <v>7.38</v>
+      </c>
+      <c r="AG25">
+        <v>3.25</v>
+      </c>
+      <c r="AH25">
+        <v>4.13</v>
+      </c>
+      <c r="AI25">
+        <v>5.5940000000000003</v>
+      </c>
+      <c r="AJ25">
+        <v>0.91720000000000002</v>
+      </c>
+      <c r="AK25">
+        <v>7.42</v>
+      </c>
+      <c r="AL25">
+        <v>1.68</v>
+      </c>
+      <c r="AM25">
+        <v>5.74</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
-      <c r="A26" t="s">
-        <v>17</v>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
       </c>
       <c r="B26">
         <v>13.2</v>
@@ -1888,19 +3728,19 @@
         <v>23.5</v>
       </c>
       <c r="D26">
-        <v>4.644</v>
+        <v>4.6440000000000001</v>
       </c>
       <c r="E26">
-        <v>4.169</v>
+        <v>4.1689999999999996</v>
       </c>
       <c r="F26">
-        <v>5.041</v>
+        <v>5.0410000000000004</v>
       </c>
       <c r="G26">
         <v>2.9</v>
       </c>
       <c r="H26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -1909,10 +3749,10 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <v>4.399999999999999</v>
+        <v>4.3999999999999986</v>
       </c>
       <c r="L26">
-        <v>36.8</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="M26">
         <v>44.1</v>
@@ -1921,15 +3761,84 @@
         <v>14.7</v>
       </c>
       <c r="O26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P26" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>60</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>40</v>
+      </c>
+      <c r="W26">
+        <v>8</v>
+      </c>
+      <c r="X26">
+        <v>8</v>
+      </c>
+      <c r="Y26">
+        <v>4.6440000000000001</v>
+      </c>
+      <c r="Z26">
+        <v>1.4931000000000001</v>
+      </c>
+      <c r="AA26">
+        <v>6.9</v>
+      </c>
+      <c r="AB26">
+        <v>1.71</v>
+      </c>
+      <c r="AC26">
+        <v>5.19</v>
+      </c>
+      <c r="AD26">
+        <v>4.1689999999999996</v>
+      </c>
+      <c r="AE26">
+        <v>0.83109999999999995</v>
+      </c>
+      <c r="AF26">
+        <v>6.02</v>
+      </c>
+      <c r="AG26">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AH26">
+        <v>3.47</v>
+      </c>
+      <c r="AI26">
+        <v>5.0410000000000004</v>
+      </c>
+      <c r="AJ26">
+        <v>1.0528</v>
+      </c>
+      <c r="AK26">
+        <v>6.84</v>
+      </c>
+      <c r="AL26">
+        <v>3.06</v>
+      </c>
+      <c r="AM26">
+        <v>3.78</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
-      <c r="A27" t="s">
-        <v>17</v>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
       </c>
       <c r="B27">
         <v>1.7</v>
@@ -1941,16 +3850,16 @@
         <v>5.343</v>
       </c>
       <c r="E27">
-        <v>4.168</v>
+        <v>4.1680000000000001</v>
       </c>
       <c r="F27">
-        <v>5.178</v>
+        <v>5.1779999999999999</v>
       </c>
       <c r="G27">
         <v>2.9</v>
       </c>
       <c r="H27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -1971,15 +3880,84 @@
         <v>18</v>
       </c>
       <c r="O27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P27" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="Q27">
+        <v>100</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>11</v>
+      </c>
+      <c r="X27">
+        <v>24</v>
+      </c>
+      <c r="Y27">
+        <v>5.343</v>
+      </c>
+      <c r="Z27">
+        <v>1.1577999999999999</v>
+      </c>
+      <c r="AA27">
+        <v>7.75</v>
+      </c>
+      <c r="AB27">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="AC27">
+        <v>5.28</v>
+      </c>
+      <c r="AD27">
+        <v>4.1680000000000001</v>
+      </c>
+      <c r="AE27">
+        <v>0.88219999999999998</v>
+      </c>
+      <c r="AF27">
+        <v>7.11</v>
+      </c>
+      <c r="AG27">
+        <v>3.09</v>
+      </c>
+      <c r="AH27">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="AI27">
+        <v>5.1779999999999999</v>
+      </c>
+      <c r="AJ27">
+        <v>0.83720000000000006</v>
+      </c>
+      <c r="AK27">
+        <v>6.89</v>
+      </c>
+      <c r="AL27">
+        <v>3.57</v>
+      </c>
+      <c r="AM27">
+        <v>3.32</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
-      <c r="A28" t="s">
-        <v>17</v>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
       </c>
       <c r="B28">
         <v>1.9</v>
@@ -1991,16 +3969,16 @@
         <v>5.234</v>
       </c>
       <c r="E28">
-        <v>4.156</v>
+        <v>4.1559999999999997</v>
       </c>
       <c r="F28">
-        <v>5.547</v>
+        <v>5.5469999999999997</v>
       </c>
       <c r="G28">
         <v>2.9</v>
       </c>
       <c r="H28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -2021,15 +3999,84 @@
         <v>9.6</v>
       </c>
       <c r="O28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="P28" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="Q28">
+        <v>100</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>5</v>
+      </c>
+      <c r="X28">
+        <v>14</v>
+      </c>
+      <c r="Y28">
+        <v>5.234</v>
+      </c>
+      <c r="Z28">
+        <v>1.3319000000000001</v>
+      </c>
+      <c r="AA28">
+        <v>7.96</v>
+      </c>
+      <c r="AB28">
+        <v>2.59</v>
+      </c>
+      <c r="AC28">
+        <v>5.37</v>
+      </c>
+      <c r="AD28">
+        <v>4.1559999999999997</v>
+      </c>
+      <c r="AE28">
+        <v>0.9123</v>
+      </c>
+      <c r="AF28">
+        <v>6.31</v>
+      </c>
+      <c r="AG28">
+        <v>2.57</v>
+      </c>
+      <c r="AH28">
+        <v>3.74</v>
+      </c>
+      <c r="AI28">
+        <v>5.5469999999999997</v>
+      </c>
+      <c r="AJ28">
+        <v>0.94710000000000005</v>
+      </c>
+      <c r="AK28">
+        <v>7.17</v>
+      </c>
+      <c r="AL28">
+        <v>3.55</v>
+      </c>
+      <c r="AM28">
+        <v>3.62</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
-      <c r="A29" t="s">
-        <v>17</v>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
       </c>
       <c r="B29">
         <v>7.1</v>
@@ -2038,19 +4085,19 @@
         <v>28.6</v>
       </c>
       <c r="D29">
-        <v>5.105</v>
+        <v>5.1050000000000004</v>
       </c>
       <c r="E29">
-        <v>4.067</v>
+        <v>4.0670000000000002</v>
       </c>
       <c r="F29">
-        <v>5.393</v>
+        <v>5.3929999999999998</v>
       </c>
       <c r="G29">
         <v>5.4</v>
       </c>
       <c r="H29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I29">
         <v>1</v>
@@ -2062,24 +4109,93 @@
         <v>8.9</v>
       </c>
       <c r="L29">
-        <v>35.7</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="M29">
-        <v>35.7</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="N29">
         <v>10.7</v>
       </c>
       <c r="O29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P29" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="Q29">
+        <v>33.33</v>
+      </c>
+      <c r="R29">
+        <v>8.33</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>41.67</v>
+      </c>
+      <c r="W29">
+        <v>18</v>
+      </c>
+      <c r="X29">
+        <v>30</v>
+      </c>
+      <c r="Y29">
+        <v>5.1050000000000004</v>
+      </c>
+      <c r="Z29">
+        <v>1.6076999999999999</v>
+      </c>
+      <c r="AA29">
+        <v>7.98</v>
+      </c>
+      <c r="AB29">
+        <v>1.71</v>
+      </c>
+      <c r="AC29">
+        <v>6.27</v>
+      </c>
+      <c r="AD29">
+        <v>4.0670000000000002</v>
+      </c>
+      <c r="AE29">
+        <v>0.77990000000000004</v>
+      </c>
+      <c r="AF29">
+        <v>6.5</v>
+      </c>
+      <c r="AG29">
+        <v>2.29</v>
+      </c>
+      <c r="AH29">
+        <v>4.21</v>
+      </c>
+      <c r="AI29">
+        <v>5.3929999999999998</v>
+      </c>
+      <c r="AJ29">
+        <v>0.96560000000000001</v>
+      </c>
+      <c r="AK29">
+        <v>6.72</v>
+      </c>
+      <c r="AL29">
+        <v>3.06</v>
+      </c>
+      <c r="AM29">
+        <v>3.66</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
-      <c r="A30" t="s">
-        <v>17</v>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0</v>
       </c>
       <c r="B30">
         <v>4.8</v>
@@ -2088,19 +4204,19 @@
         <v>21.2</v>
       </c>
       <c r="D30">
-        <v>5.238</v>
+        <v>5.2380000000000004</v>
       </c>
       <c r="E30">
-        <v>4.323</v>
+        <v>4.3230000000000004</v>
       </c>
       <c r="F30">
-        <v>5.434</v>
+        <v>5.4340000000000002</v>
       </c>
       <c r="G30">
         <v>3.8</v>
       </c>
       <c r="H30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -2121,15 +4237,84 @@
         <v>10.1</v>
       </c>
       <c r="O30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P30" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="Q30">
+        <v>50</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>25</v>
+      </c>
+      <c r="T30">
+        <v>12.5</v>
+      </c>
+      <c r="U30">
+        <v>12.5</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>15</v>
+      </c>
+      <c r="X30">
+        <v>29</v>
+      </c>
+      <c r="Y30">
+        <v>5.21</v>
+      </c>
+      <c r="Z30">
+        <v>1.5092000000000001</v>
+      </c>
+      <c r="AA30">
+        <v>7.95</v>
+      </c>
+      <c r="AB30">
+        <v>1.67</v>
+      </c>
+      <c r="AC30">
+        <v>6.28</v>
+      </c>
+      <c r="AD30">
+        <v>4.32</v>
+      </c>
+      <c r="AE30">
+        <v>0.9284</v>
+      </c>
+      <c r="AF30">
+        <v>6.81</v>
+      </c>
+      <c r="AG30">
+        <v>2.7</v>
+      </c>
+      <c r="AH30">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="AI30">
+        <v>5.431</v>
+      </c>
+      <c r="AJ30">
+        <v>1.0557000000000001</v>
+      </c>
+      <c r="AK30">
+        <v>6.88</v>
+      </c>
+      <c r="AL30">
+        <v>2.96</v>
+      </c>
+      <c r="AM30">
+        <v>3.92</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
-      <c r="A31" t="s">
-        <v>17</v>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0</v>
       </c>
       <c r="B31">
         <v>6.9</v>
@@ -2141,16 +4326,16 @@
         <v>5.423</v>
       </c>
       <c r="E31">
-        <v>4.095</v>
+        <v>4.0949999999999998</v>
       </c>
       <c r="F31">
-        <v>5.504</v>
+        <v>5.5039999999999996</v>
       </c>
       <c r="G31">
-        <v>4.100000000000001</v>
+        <v>4.1000000000000014</v>
       </c>
       <c r="H31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I31">
         <v>1</v>
@@ -2159,22 +4344,91 @@
         <v>1</v>
       </c>
       <c r="K31">
-        <v>6.600000000000001</v>
+        <v>6.6000000000000014</v>
       </c>
       <c r="L31">
-        <v>36.2</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="M31">
-        <v>39.3</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="N31">
         <v>9</v>
       </c>
       <c r="O31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P31" t="s">
-        <v>91</v>
+        <v>89</v>
+      </c>
+      <c r="Q31">
+        <v>31.58</v>
+      </c>
+      <c r="R31">
+        <v>10.53</v>
+      </c>
+      <c r="S31">
+        <v>26.32</v>
+      </c>
+      <c r="T31">
+        <v>15.79</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <v>15.79</v>
+      </c>
+      <c r="W31">
+        <v>17</v>
+      </c>
+      <c r="X31">
+        <v>30</v>
+      </c>
+      <c r="Y31">
+        <v>5.423</v>
+      </c>
+      <c r="Z31">
+        <v>1.1484000000000001</v>
+      </c>
+      <c r="AA31">
+        <v>7.86</v>
+      </c>
+      <c r="AB31">
+        <v>2.02</v>
+      </c>
+      <c r="AC31">
+        <v>5.84</v>
+      </c>
+      <c r="AD31">
+        <v>4.0949999999999998</v>
+      </c>
+      <c r="AE31">
+        <v>0.85350000000000004</v>
+      </c>
+      <c r="AF31">
+        <v>6.6</v>
+      </c>
+      <c r="AG31">
+        <v>2.15</v>
+      </c>
+      <c r="AH31">
+        <v>4.45</v>
+      </c>
+      <c r="AI31">
+        <v>5.5039999999999996</v>
+      </c>
+      <c r="AJ31">
+        <v>0.74909999999999999</v>
+      </c>
+      <c r="AK31">
+        <v>7</v>
+      </c>
+      <c r="AL31">
+        <v>3.2</v>
+      </c>
+      <c r="AM31">
+        <v>3.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>